<commit_message>
Added more test data to spreadsheet
</commit_message>
<xml_diff>
--- a/RichAutomationDemo/src/test/resources/test_data_for_POST.xlsx
+++ b/RichAutomationDemo/src/test/resources/test_data_for_POST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\IdeaProjects\RichAutomationDemo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACED5E4-ACFE-497C-B0A3-798DC22F509A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC9741A-3054-4E29-9F7A-09B7563F79B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37DC7992-922F-4566-9A2A-5170C9386B1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -53,52 +53,86 @@
     <t>status</t>
   </si>
   <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>tyfh@gm.com</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>Tony SPLIZ</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>John Blon</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>hello@hg.com</t>
-  </si>
-  <si>
-    <t>Joey Bonzo</t>
-  </si>
-  <si>
-    <t>hello@geh.com</t>
+    <t>Tony Spliz</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>tony.spliz@test.com</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Maria Chen</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>maria.chen@test.com</t>
+  </si>
+  <si>
+    <t>Leo Martinez</t>
+  </si>
+  <si>
+    <t>leo.m@test.com</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Priya Kapoor</t>
+  </si>
+  <si>
+    <t>priya.k@test.com</t>
+  </si>
+  <si>
+    <t>Ahmed Zahir</t>
+  </si>
+  <si>
+    <t>ahmed.z@test.com</t>
+  </si>
+  <si>
+    <t>Chloe Bennett</t>
+  </si>
+  <si>
+    <t>chloe.b@test.com</t>
+  </si>
+  <si>
+    <t>Rajiv Patel</t>
+  </si>
+  <si>
+    <t>rajiv.p@test.com</t>
+  </si>
+  <si>
+    <t>Emily Tran</t>
+  </si>
+  <si>
+    <t>emily.tran@test.com</t>
+  </si>
+  <si>
+    <t>Marcus Lee</t>
+  </si>
+  <si>
+    <t>marcus.lee@test.com</t>
+  </si>
+  <si>
+    <t>Sofia Alvarez</t>
+  </si>
+  <si>
+    <t>sofia.a@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,17 +155,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B679D1E-1B59-4848-89E4-A68AACBD7192}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,57 +529,147 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{1B5AF7C3-B9C5-416B-8B79-2BB0EA71CA92}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{A6979F2B-83CE-47AD-9BDD-3361D68B173F}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{015F0A6C-C5E3-4227-9838-23A1CA0F2DFF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>